<commit_message>
fixed date for comtrade data
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021A.xlsx
+++ b/data/comtrade_total_exports_2021A.xlsx
@@ -15,6 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -52,11 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,11 +355,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
@@ -365,7 +372,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>refPeriodId</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -414,11 +421,6 @@
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>cmdDesc</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>primaryValue</t>
         </is>
@@ -430,8 +432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B2">
-        <v>20210101</v>
+      <c r="B2" s="2">
+        <v>44197</v>
       </c>
       <c r="C2">
         <v>2021</v>
@@ -470,12 +472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M2">
+      <c r="L2">
         <v>163974317.51</v>
       </c>
     </row>
@@ -485,8 +482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B3">
-        <v>20210101</v>
+      <c r="B3" s="2">
+        <v>44197</v>
       </c>
       <c r="C3">
         <v>2021</v>
@@ -525,12 +522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M3">
+      <c r="L3">
         <v>33260057816.965</v>
       </c>
     </row>
@@ -540,8 +532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B4">
-        <v>20210101</v>
+      <c r="B4" s="2">
+        <v>44197</v>
       </c>
       <c r="C4">
         <v>2021</v>
@@ -580,12 +572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M4">
+      <c r="L4">
         <v>22207974784.94</v>
       </c>
     </row>
@@ -595,8 +582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B5">
-        <v>20210101</v>
+      <c r="B5" s="2">
+        <v>44197</v>
       </c>
       <c r="C5">
         <v>2021</v>
@@ -635,12 +622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M5">
+      <c r="L5">
         <v>77934314986.58</v>
       </c>
     </row>
@@ -650,8 +632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B6">
-        <v>20210101</v>
+      <c r="B6" s="2">
+        <v>44197</v>
       </c>
       <c r="C6">
         <v>2021</v>
@@ -690,12 +672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M6">
+      <c r="L6">
         <v>342036103269.844</v>
       </c>
     </row>
@@ -705,8 +682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B7">
-        <v>20210101</v>
+      <c r="B7" s="2">
+        <v>44197</v>
       </c>
       <c r="C7">
         <v>2021</v>
@@ -745,12 +722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M7">
+      <c r="L7">
         <v>201647281767.755</v>
       </c>
     </row>
@@ -760,8 +732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B8">
-        <v>20210101</v>
+      <c r="B8" s="2">
+        <v>44197</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -800,12 +772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M8">
+      <c r="L8">
         <v>2964798290.08</v>
       </c>
     </row>
@@ -815,8 +782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B9">
-        <v>20210101</v>
+      <c r="B9" s="2">
+        <v>44197</v>
       </c>
       <c r="C9">
         <v>2021</v>
@@ -855,12 +822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M9">
+      <c r="L9">
         <v>350172911</v>
       </c>
     </row>
@@ -870,8 +832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B10">
-        <v>20210101</v>
+      <c r="B10" s="2">
+        <v>44197</v>
       </c>
       <c r="C10">
         <v>2021</v>
@@ -910,12 +872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M10">
+      <c r="L10">
         <v>386354055203.238</v>
       </c>
     </row>
@@ -925,8 +882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B11">
-        <v>20210101</v>
+      <c r="B11" s="2">
+        <v>44197</v>
       </c>
       <c r="C11">
         <v>2021</v>
@@ -965,12 +922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M11">
+      <c r="L11">
         <v>28632529.08</v>
       </c>
     </row>
@@ -980,8 +932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B12">
-        <v>20210101</v>
+      <c r="B12" s="2">
+        <v>44197</v>
       </c>
       <c r="C12">
         <v>2021</v>
@@ -1020,12 +972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M12">
+      <c r="L12">
         <v>11079788840.24</v>
       </c>
     </row>
@@ -1035,8 +982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B13">
-        <v>20210101</v>
+      <c r="B13" s="2">
+        <v>44197</v>
       </c>
       <c r="C13">
         <v>2021</v>
@@ -1075,12 +1022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M13">
+      <c r="L13">
         <v>8614110010.865999</v>
       </c>
     </row>
@@ -1090,8 +1032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B14">
-        <v>20210101</v>
+      <c r="B14" s="2">
+        <v>44197</v>
       </c>
       <c r="C14">
         <v>2021</v>
@@ -1130,12 +1072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M14">
+      <c r="L14">
         <v>7473466757.015</v>
       </c>
     </row>
@@ -1145,8 +1082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B15">
-        <v>20210101</v>
+      <c r="B15" s="2">
+        <v>44197</v>
       </c>
       <c r="C15">
         <v>2021</v>
@@ -1185,12 +1122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M15">
+      <c r="L15">
         <v>280814577460</v>
       </c>
     </row>
@@ -1200,8 +1132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B16">
-        <v>20210101</v>
+      <c r="B16" s="2">
+        <v>44197</v>
       </c>
       <c r="C16">
         <v>2021</v>
@@ -1240,12 +1172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M16">
+      <c r="L16">
         <v>264092675.61</v>
       </c>
     </row>
@@ -1255,8 +1182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B17">
-        <v>20210101</v>
+      <c r="B17" s="2">
+        <v>44197</v>
       </c>
       <c r="C17">
         <v>2021</v>
@@ -1295,12 +1222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M17">
+      <c r="L17">
         <v>11058184373.01</v>
       </c>
     </row>
@@ -1310,8 +1232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B18">
-        <v>20210101</v>
+      <c r="B18" s="2">
+        <v>44197</v>
       </c>
       <c r="C18">
         <v>2021</v>
@@ -1350,12 +1272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M18">
+      <c r="L18">
         <v>41370856687.293</v>
       </c>
     </row>
@@ -1365,8 +1282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B19">
-        <v>20210101</v>
+      <c r="B19" s="2">
+        <v>44197</v>
       </c>
       <c r="C19">
         <v>2021</v>
@@ -1405,12 +1322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M19">
+      <c r="L19">
         <v>15144859129.46</v>
       </c>
     </row>
@@ -1420,8 +1332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B20">
-        <v>20210101</v>
+      <c r="B20" s="2">
+        <v>44197</v>
       </c>
       <c r="C20">
         <v>2021</v>
@@ -1460,12 +1372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M20">
+      <c r="L20">
         <v>113150402.25</v>
       </c>
     </row>
@@ -1475,8 +1382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B21">
-        <v>20210101</v>
+      <c r="B21" s="2">
+        <v>44197</v>
       </c>
       <c r="C21">
         <v>2021</v>
@@ -1515,12 +1422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M21">
+      <c r="L21">
         <v>39889022800</v>
       </c>
     </row>
@@ -1530,8 +1432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B22">
-        <v>20210101</v>
+      <c r="B22" s="2">
+        <v>44197</v>
       </c>
       <c r="C22">
         <v>2021</v>
@@ -1570,12 +1472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M22">
+      <c r="L22">
         <v>17571782672.48</v>
       </c>
     </row>
@@ -1585,8 +1482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B23">
-        <v>20210101</v>
+      <c r="B23" s="2">
+        <v>44197</v>
       </c>
       <c r="C23">
         <v>2021</v>
@@ -1625,12 +1522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M23">
+      <c r="L23">
         <v>501463001508.414</v>
       </c>
     </row>
@@ -1640,8 +1532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B24">
-        <v>20210101</v>
+      <c r="B24" s="2">
+        <v>44197</v>
       </c>
       <c r="C24">
         <v>2021</v>
@@ -1680,12 +1572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M24">
+      <c r="L24">
         <v>17082261.232</v>
       </c>
     </row>
@@ -1695,8 +1582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B25">
-        <v>20210101</v>
+      <c r="B25" s="2">
+        <v>44197</v>
       </c>
       <c r="C25">
         <v>2021</v>
@@ -1735,12 +1622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M25">
+      <c r="L25">
         <v>13331248583.322</v>
       </c>
     </row>
@@ -1750,8 +1632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B26">
-        <v>20210101</v>
+      <c r="B26" s="2">
+        <v>44197</v>
       </c>
       <c r="C26">
         <v>2021</v>
@@ -1790,12 +1672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M26">
+      <c r="L26">
         <v>94676809206.28101</v>
       </c>
     </row>
@@ -1805,8 +1682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B27">
-        <v>20210101</v>
+      <c r="B27" s="2">
+        <v>44197</v>
       </c>
       <c r="C27">
         <v>2021</v>
@@ -1845,12 +1722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M27">
+      <c r="L27">
         <v>3362301613439</v>
       </c>
     </row>
@@ -1860,8 +1732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B28">
-        <v>20210101</v>
+      <c r="B28" s="2">
+        <v>44197</v>
       </c>
       <c r="C28">
         <v>2021</v>
@@ -1900,12 +1772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M28">
+      <c r="L28">
         <v>41389989047.59</v>
       </c>
     </row>
@@ -1915,8 +1782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B29">
-        <v>20210101</v>
+      <c r="B29" s="2">
+        <v>44197</v>
       </c>
       <c r="C29">
         <v>2021</v>
@@ -1955,12 +1822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M29">
+      <c r="L29">
         <v>34994132.52</v>
       </c>
     </row>
@@ -1970,8 +1832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B30">
-        <v>20210101</v>
+      <c r="B30" s="2">
+        <v>44197</v>
       </c>
       <c r="C30">
         <v>2021</v>
@@ -2010,12 +1872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M30">
+      <c r="L30">
         <v>2362230161.01</v>
       </c>
     </row>
@@ -2025,8 +1882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B31">
-        <v>20210101</v>
+      <c r="B31" s="2">
+        <v>44197</v>
       </c>
       <c r="C31">
         <v>2021</v>
@@ -2065,12 +1922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M31">
+      <c r="L31">
         <v>14345395565.22</v>
       </c>
     </row>
@@ -2080,8 +1932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B32">
-        <v>20210101</v>
+      <c r="B32" s="2">
+        <v>44197</v>
       </c>
       <c r="C32">
         <v>2021</v>
@@ -2120,12 +1972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M32">
+      <c r="L32">
         <v>21827948964</v>
       </c>
     </row>
@@ -2135,8 +1982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B33">
-        <v>20210101</v>
+      <c r="B33" s="2">
+        <v>44197</v>
       </c>
       <c r="C33">
         <v>2021</v>
@@ -2175,12 +2022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M33">
+      <c r="L33">
         <v>3989812264.347</v>
       </c>
     </row>
@@ -2190,8 +2032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B34">
-        <v>20210101</v>
+      <c r="B34" s="2">
+        <v>44197</v>
       </c>
       <c r="C34">
         <v>2021</v>
@@ -2230,12 +2072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M34">
+      <c r="L34">
         <v>227168411022</v>
       </c>
     </row>
@@ -2245,8 +2082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B35">
-        <v>20210101</v>
+      <c r="B35" s="2">
+        <v>44197</v>
       </c>
       <c r="C35">
         <v>2021</v>
@@ -2285,12 +2122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M35">
+      <c r="L35">
         <v>1023522023.899</v>
       </c>
     </row>
@@ -2300,8 +2132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B36">
-        <v>20210101</v>
+      <c r="B36" s="2">
+        <v>44197</v>
       </c>
       <c r="C36">
         <v>2021</v>
@@ -2340,12 +2172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M36">
+      <c r="L36">
         <v>125014614347.861</v>
       </c>
     </row>
@@ -2355,8 +2182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B37">
-        <v>20210101</v>
+      <c r="B37" s="2">
+        <v>44197</v>
       </c>
       <c r="C37">
         <v>2021</v>
@@ -2395,12 +2222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M37">
+      <c r="L37">
         <v>11725013719.98</v>
       </c>
     </row>
@@ -2410,8 +2232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B38">
-        <v>20210101</v>
+      <c r="B38" s="2">
+        <v>44197</v>
       </c>
       <c r="C38">
         <v>2021</v>
@@ -2450,12 +2272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M38">
+      <c r="L38">
         <v>26699199844.372</v>
       </c>
     </row>
@@ -2465,8 +2282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B39">
-        <v>20210101</v>
+      <c r="B39" s="2">
+        <v>44197</v>
       </c>
       <c r="C39">
         <v>2021</v>
@@ -2505,12 +2322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M39">
+      <c r="L39">
         <v>6394888915.91</v>
       </c>
     </row>
@@ -2520,8 +2332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B40">
-        <v>20210101</v>
+      <c r="B40" s="2">
+        <v>44197</v>
       </c>
       <c r="C40">
         <v>2021</v>
@@ -2560,12 +2372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M40">
+      <c r="L40">
         <v>3057628826.59</v>
       </c>
     </row>
@@ -2575,8 +2382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B41">
-        <v>20210101</v>
+      <c r="B41" s="2">
+        <v>44197</v>
       </c>
       <c r="C41">
         <v>2021</v>
@@ -2615,12 +2422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M41">
+      <c r="L41">
         <v>22282223314.05</v>
       </c>
     </row>
@@ -2630,8 +2432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B42">
-        <v>20210101</v>
+      <c r="B42" s="2">
+        <v>44197</v>
       </c>
       <c r="C42">
         <v>2021</v>
@@ -2670,12 +2472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M42">
+      <c r="L42">
         <v>815335653.153</v>
       </c>
     </row>
@@ -2685,8 +2482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B43">
-        <v>20210101</v>
+      <c r="B43" s="2">
+        <v>44197</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -2725,12 +2522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M43">
+      <c r="L43">
         <v>81500265209.30499</v>
       </c>
     </row>
@@ -2740,8 +2532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B44">
-        <v>20210101</v>
+      <c r="B44" s="2">
+        <v>44197</v>
       </c>
       <c r="C44">
         <v>2021</v>
@@ -2780,12 +2572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M44">
+      <c r="L44">
         <v>585148036598.849</v>
       </c>
     </row>
@@ -2795,8 +2582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B45">
-        <v>20210101</v>
+      <c r="B45" s="2">
+        <v>44197</v>
       </c>
       <c r="C45">
         <v>2021</v>
@@ -2835,12 +2622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M45">
+      <c r="L45">
         <v>4242653017.17</v>
       </c>
     </row>
@@ -2850,8 +2632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B46">
-        <v>20210101</v>
+      <c r="B46" s="2">
+        <v>44197</v>
       </c>
       <c r="C46">
         <v>2021</v>
@@ -2890,12 +2672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M46">
+      <c r="L46">
         <v>26401460.44</v>
       </c>
     </row>
@@ -2905,8 +2682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B47">
-        <v>20210101</v>
+      <c r="B47" s="2">
+        <v>44197</v>
       </c>
       <c r="C47">
         <v>2021</v>
@@ -2945,12 +2722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M47">
+      <c r="L47">
         <v>1357640029.17</v>
       </c>
     </row>
@@ -2960,8 +2732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B48">
-        <v>20210101</v>
+      <c r="B48" s="2">
+        <v>44197</v>
       </c>
       <c r="C48">
         <v>2021</v>
@@ -3000,12 +2772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M48">
+      <c r="L48">
         <v>1635599573787.609</v>
       </c>
     </row>
@@ -3015,8 +2782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B49">
-        <v>20210101</v>
+      <c r="B49" s="2">
+        <v>44197</v>
       </c>
       <c r="C49">
         <v>2021</v>
@@ -3055,12 +2822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M49">
+      <c r="L49">
         <v>47244277316.697</v>
       </c>
     </row>
@@ -3070,8 +2832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B50">
-        <v>20210101</v>
+      <c r="B50" s="2">
+        <v>44197</v>
       </c>
       <c r="C50">
         <v>2021</v>
@@ -3110,12 +2872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M50">
+      <c r="L50">
         <v>35163394.409</v>
       </c>
     </row>
@@ -3125,8 +2882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B51">
-        <v>20210101</v>
+      <c r="B51" s="2">
+        <v>44197</v>
       </c>
       <c r="C51">
         <v>2021</v>
@@ -3165,12 +2922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M51">
+      <c r="L51">
         <v>13735599195</v>
       </c>
     </row>
@@ -3180,8 +2932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B52">
-        <v>20210101</v>
+      <c r="B52" s="2">
+        <v>44197</v>
       </c>
       <c r="C52">
         <v>2021</v>
@@ -3220,12 +2972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M52">
+      <c r="L52">
         <v>4257250461.689</v>
       </c>
     </row>
@@ -3235,8 +2982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B53">
-        <v>20210101</v>
+      <c r="B53" s="2">
+        <v>44197</v>
       </c>
       <c r="C53">
         <v>2021</v>
@@ -3275,12 +3022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M53">
+      <c r="L53">
         <v>4975948988.14</v>
       </c>
     </row>
@@ -3290,8 +3032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B54">
-        <v>20210101</v>
+      <c r="B54" s="2">
+        <v>44197</v>
       </c>
       <c r="C54">
         <v>2021</v>
@@ -3330,12 +3072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M54">
+      <c r="L54">
         <v>670926079457.053</v>
       </c>
     </row>
@@ -3345,8 +3082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B55">
-        <v>20210101</v>
+      <c r="B55" s="2">
+        <v>44197</v>
       </c>
       <c r="C55">
         <v>2021</v>
@@ -3385,12 +3122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M55">
+      <c r="L55">
         <v>141157091681</v>
       </c>
     </row>
@@ -3400,8 +3132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B56">
-        <v>20210101</v>
+      <c r="B56" s="2">
+        <v>44197</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -3440,12 +3172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M56">
+      <c r="L56">
         <v>5973742650.46</v>
       </c>
     </row>
@@ -3455,8 +3182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B57">
-        <v>20210101</v>
+      <c r="B57" s="2">
+        <v>44197</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -3495,12 +3222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M57">
+      <c r="L57">
         <v>231522458128.8</v>
       </c>
     </row>
@@ -3510,8 +3232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B58">
-        <v>20210101</v>
+      <c r="B58" s="2">
+        <v>44197</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -3550,12 +3272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M58">
+      <c r="L58">
         <v>195997875900.844</v>
       </c>
     </row>
@@ -3565,8 +3282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B59">
-        <v>20210101</v>
+      <c r="B59" s="2">
+        <v>44197</v>
       </c>
       <c r="C59">
         <v>2021</v>
@@ -3605,12 +3322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M59">
+      <c r="L59">
         <v>60159734000</v>
       </c>
     </row>
@@ -3620,8 +3332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B60">
-        <v>20210101</v>
+      <c r="B60" s="2">
+        <v>44197</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -3660,12 +3372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M60">
+      <c r="L60">
         <v>615910260060.774</v>
       </c>
     </row>
@@ -3675,8 +3382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B61">
-        <v>20210101</v>
+      <c r="B61" s="2">
+        <v>44197</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -3715,12 +3422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M61">
+      <c r="L61">
         <v>1440530765.28</v>
       </c>
     </row>
@@ -3730,8 +3432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B62">
-        <v>20210101</v>
+      <c r="B62" s="2">
+        <v>44197</v>
       </c>
       <c r="C62">
         <v>2021</v>
@@ -3770,12 +3472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M62">
+      <c r="L62">
         <v>757066261248.9709</v>
       </c>
     </row>
@@ -3785,8 +3482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B63">
-        <v>20210101</v>
+      <c r="B63" s="2">
+        <v>44197</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -3825,12 +3522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M63">
+      <c r="L63">
         <v>9356550020.493999</v>
       </c>
     </row>
@@ -3840,8 +3532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B64">
-        <v>20210101</v>
+      <c r="B64" s="2">
+        <v>44197</v>
       </c>
       <c r="C64">
         <v>2021</v>
@@ -3880,12 +3572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M64">
+      <c r="L64">
         <v>6751366221.034</v>
       </c>
     </row>
@@ -3895,8 +3582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B65">
-        <v>20210101</v>
+      <c r="B65" s="2">
+        <v>44197</v>
       </c>
       <c r="C65">
         <v>2021</v>
@@ -3935,12 +3622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M65">
+      <c r="L65">
         <v>644411147014</v>
       </c>
     </row>
@@ -3950,8 +3632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B66">
-        <v>20210101</v>
+      <c r="B66" s="2">
+        <v>44197</v>
       </c>
       <c r="C66">
         <v>2021</v>
@@ -3990,12 +3672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M66">
+      <c r="L66">
         <v>63129693952</v>
       </c>
     </row>
@@ -4005,8 +3682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B67">
-        <v>20210101</v>
+      <c r="B67" s="2">
+        <v>44197</v>
       </c>
       <c r="C67">
         <v>2021</v>
@@ -4045,12 +3722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M67">
+      <c r="L67">
         <v>2752163636</v>
       </c>
     </row>
@@ -4060,8 +3732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B68">
-        <v>20210101</v>
+      <c r="B68" s="2">
+        <v>44197</v>
       </c>
       <c r="C68">
         <v>2021</v>
@@ -4100,12 +3772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M68">
+      <c r="L68">
         <v>7164605459.07</v>
       </c>
     </row>
@@ -4115,8 +3782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B69">
-        <v>20210101</v>
+      <c r="B69" s="2">
+        <v>44197</v>
       </c>
       <c r="C69">
         <v>2021</v>
@@ -4155,12 +3822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M69">
+      <c r="L69">
         <v>4229976738</v>
       </c>
     </row>
@@ -4170,8 +3832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B70">
-        <v>20210101</v>
+      <c r="B70" s="2">
+        <v>44197</v>
       </c>
       <c r="C70">
         <v>2021</v>
@@ -4210,12 +3872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M70">
+      <c r="L70">
         <v>948535188.45</v>
       </c>
     </row>
@@ -4225,8 +3882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B71">
-        <v>20210101</v>
+      <c r="B71" s="2">
+        <v>44197</v>
       </c>
       <c r="C71">
         <v>2021</v>
@@ -4265,12 +3922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M71">
+      <c r="L71">
         <v>19458821916.273</v>
       </c>
     </row>
@@ -4280,8 +3932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B72">
-        <v>20210101</v>
+      <c r="B72" s="2">
+        <v>44197</v>
       </c>
       <c r="C72">
         <v>2021</v>
@@ -4320,12 +3972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M72">
+      <c r="L72">
         <v>40698383278.78</v>
       </c>
     </row>
@@ -4335,8 +3982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B73">
-        <v>20210101</v>
+      <c r="B73" s="2">
+        <v>44197</v>
       </c>
       <c r="C73">
         <v>2021</v>
@@ -4375,12 +4022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M73">
+      <c r="L73">
         <v>16247126542.139</v>
       </c>
     </row>
@@ -4390,8 +4032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B74">
-        <v>20210101</v>
+      <c r="B74" s="2">
+        <v>44197</v>
       </c>
       <c r="C74">
         <v>2021</v>
@@ -4430,12 +4072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M74">
+      <c r="L74">
         <v>1392424900.553</v>
       </c>
     </row>
@@ -4445,8 +4082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B75">
-        <v>20210101</v>
+      <c r="B75" s="2">
+        <v>44197</v>
       </c>
       <c r="C75">
         <v>2021</v>
@@ -4485,12 +4122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M75">
+      <c r="L75">
         <v>2788376340.521</v>
       </c>
     </row>
@@ -4500,8 +4132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B76">
-        <v>20210101</v>
+      <c r="B76" s="2">
+        <v>44197</v>
       </c>
       <c r="C76">
         <v>2021</v>
@@ -4540,12 +4172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M76">
+      <c r="L76">
         <v>299230434394.232</v>
       </c>
     </row>
@@ -4555,8 +4182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B77">
-        <v>20210101</v>
+      <c r="B77" s="2">
+        <v>44197</v>
       </c>
       <c r="C77">
         <v>2021</v>
@@ -4595,12 +4222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M77">
+      <c r="L77">
         <v>151293266.49</v>
       </c>
     </row>
@@ -4610,8 +4232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B78">
-        <v>20210101</v>
+      <c r="B78" s="2">
+        <v>44197</v>
       </c>
       <c r="C78">
         <v>2021</v>
@@ -4650,12 +4272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M78">
+      <c r="L78">
         <v>3200429629.51</v>
       </c>
     </row>
@@ -4665,8 +4282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B79">
-        <v>20210101</v>
+      <c r="B79" s="2">
+        <v>44197</v>
       </c>
       <c r="C79">
         <v>2021</v>
@@ -4705,12 +4322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M79">
+      <c r="L79">
         <v>3266988807.55</v>
       </c>
     </row>
@@ -4720,8 +4332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B80">
-        <v>20210101</v>
+      <c r="B80" s="2">
+        <v>44197</v>
       </c>
       <c r="C80">
         <v>2021</v>
@@ -4760,12 +4372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M80">
+      <c r="L80">
         <v>1671760288.267</v>
       </c>
     </row>
@@ -4775,8 +4382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B81">
-        <v>20210101</v>
+      <c r="B81" s="2">
+        <v>44197</v>
       </c>
       <c r="C81">
         <v>2021</v>
@@ -4815,12 +4422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M81">
+      <c r="L81">
         <v>494595503435</v>
       </c>
     </row>
@@ -4830,8 +4432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B82">
-        <v>20210101</v>
+      <c r="B82" s="2">
+        <v>44197</v>
       </c>
       <c r="C82">
         <v>2021</v>
@@ -4870,12 +4472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M82">
+      <c r="L82">
         <v>447656546120.094</v>
       </c>
     </row>
@@ -4885,8 +4482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B83">
-        <v>20210101</v>
+      <c r="B83" s="2">
+        <v>44197</v>
       </c>
       <c r="C83">
         <v>2021</v>
@@ -4925,12 +4522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M83">
+      <c r="L83">
         <v>9241123149.940001</v>
       </c>
     </row>
@@ -4940,8 +4532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B84">
-        <v>20210101</v>
+      <c r="B84" s="2">
+        <v>44197</v>
       </c>
       <c r="C84">
         <v>2021</v>
@@ -4980,12 +4572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M84">
+      <c r="L84">
         <v>3144504817</v>
       </c>
     </row>
@@ -4995,8 +4582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B85">
-        <v>20210101</v>
+      <c r="B85" s="2">
+        <v>44197</v>
       </c>
       <c r="C85">
         <v>2021</v>
@@ -5035,12 +4622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M85">
+      <c r="L85">
         <v>515916303.811</v>
       </c>
     </row>
@@ -5050,8 +4632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B86">
-        <v>20210101</v>
+      <c r="B86" s="2">
+        <v>44197</v>
       </c>
       <c r="C86">
         <v>2021</v>
@@ -5090,12 +4672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M86">
+      <c r="L86">
         <v>36585224951.204</v>
       </c>
     </row>
@@ -5105,8 +4682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B87">
-        <v>20210101</v>
+      <c r="B87" s="2">
+        <v>44197</v>
       </c>
       <c r="C87">
         <v>2021</v>
@@ -5145,12 +4722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M87">
+      <c r="L87">
         <v>5111685900.99</v>
       </c>
     </row>
@@ -5160,8 +4732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B88">
-        <v>20210101</v>
+      <c r="B88" s="2">
+        <v>44197</v>
       </c>
       <c r="C88">
         <v>2021</v>
@@ -5200,12 +4772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M88">
+      <c r="L88">
         <v>44590926520.592</v>
       </c>
     </row>
@@ -5215,8 +4782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B89">
-        <v>20210101</v>
+      <c r="B89" s="2">
+        <v>44197</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -5255,12 +4822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M89">
+      <c r="L89">
         <v>1665727794.55</v>
       </c>
     </row>
@@ -5270,8 +4832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B90">
-        <v>20210101</v>
+      <c r="B90" s="2">
+        <v>44197</v>
       </c>
       <c r="C90">
         <v>2021</v>
@@ -5310,12 +4872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M90">
+      <c r="L90">
         <v>696873257184.973</v>
       </c>
     </row>
@@ -5325,8 +4882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B91">
-        <v>20210101</v>
+      <c r="B91" s="2">
+        <v>44197</v>
       </c>
       <c r="C91">
         <v>2021</v>
@@ -5365,12 +4922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M91">
+      <c r="L91">
         <v>88347007.693</v>
       </c>
     </row>
@@ -5380,8 +4932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B92">
-        <v>20210101</v>
+      <c r="B92" s="2">
+        <v>44197</v>
       </c>
       <c r="C92">
         <v>2021</v>
@@ -5420,12 +4972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M92">
+      <c r="L92">
         <v>44325287820.466</v>
       </c>
     </row>
@@ -5435,8 +4982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B93">
-        <v>20210101</v>
+      <c r="B93" s="2">
+        <v>44197</v>
       </c>
       <c r="C93">
         <v>2021</v>
@@ -5475,12 +5022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M93">
+      <c r="L93">
         <v>6494984866.92</v>
       </c>
     </row>
@@ -5490,8 +5032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B94">
-        <v>20210101</v>
+      <c r="B94" s="2">
+        <v>44197</v>
       </c>
       <c r="C94">
         <v>2021</v>
@@ -5530,12 +5072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M94">
+      <c r="L94">
         <v>506672560.08</v>
       </c>
     </row>
@@ -5545,8 +5082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B95">
-        <v>20210101</v>
+      <c r="B95" s="2">
+        <v>44197</v>
       </c>
       <c r="C95">
         <v>2021</v>
@@ -5585,12 +5122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M95">
+      <c r="L95">
         <v>47231712930.364</v>
       </c>
     </row>
@@ -5600,8 +5132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B96">
-        <v>20210101</v>
+      <c r="B96" s="2">
+        <v>44197</v>
       </c>
       <c r="C96">
         <v>2021</v>
@@ -5640,12 +5172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M96">
+      <c r="L96">
         <v>161686747944.171</v>
       </c>
     </row>
@@ -5655,8 +5182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B97">
-        <v>20210101</v>
+      <c r="B97" s="2">
+        <v>44197</v>
       </c>
       <c r="C97">
         <v>2021</v>
@@ -5695,12 +5222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M97">
+      <c r="L97">
         <v>28795179085.962</v>
       </c>
     </row>
@@ -5710,8 +5232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B98">
-        <v>20210101</v>
+      <c r="B98" s="2">
+        <v>44197</v>
       </c>
       <c r="C98">
         <v>2021</v>
@@ -5750,12 +5272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M98">
+      <c r="L98">
         <v>3781922651</v>
       </c>
     </row>
@@ -5765,8 +5282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B99">
-        <v>20210101</v>
+      <c r="B99" s="2">
+        <v>44197</v>
       </c>
       <c r="C99">
         <v>2021</v>
@@ -5805,12 +5322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M99">
+      <c r="L99">
         <v>10570969868</v>
       </c>
     </row>
@@ -5820,8 +5332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B100">
-        <v>20210101</v>
+      <c r="B100" s="2">
+        <v>44197</v>
       </c>
       <c r="C100">
         <v>2021</v>
@@ -5860,12 +5372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M100">
+      <c r="L100">
         <v>56260115202.756</v>
       </c>
     </row>
@@ -5875,8 +5382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B101">
-        <v>20210101</v>
+      <c r="B101" s="2">
+        <v>44197</v>
       </c>
       <c r="C101">
         <v>2021</v>
@@ -5915,12 +5422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M101">
+      <c r="L101">
         <v>74619528755</v>
       </c>
     </row>
@@ -5930,8 +5432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B102">
-        <v>20210101</v>
+      <c r="B102" s="2">
+        <v>44197</v>
       </c>
       <c r="C102">
         <v>2021</v>
@@ -5970,12 +5472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M102">
+      <c r="L102">
         <v>317832124942</v>
       </c>
     </row>
@@ -5985,8 +5482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B103">
-        <v>20210101</v>
+      <c r="B103" s="2">
+        <v>44197</v>
       </c>
       <c r="C103">
         <v>2021</v>
@@ -6025,12 +5522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M103">
+      <c r="L103">
         <v>75242766894.064</v>
       </c>
     </row>
@@ -6040,8 +5532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B104">
-        <v>20210101</v>
+      <c r="B104" s="2">
+        <v>44197</v>
       </c>
       <c r="C104">
         <v>2021</v>
@@ -6080,12 +5572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M104">
+      <c r="L104">
         <v>87203291188.87</v>
       </c>
     </row>
@@ -6095,8 +5582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B105">
-        <v>20210101</v>
+      <c r="B105" s="2">
+        <v>44197</v>
       </c>
       <c r="C105">
         <v>2021</v>
@@ -6135,12 +5622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M105">
+      <c r="L105">
         <v>88389728970.91</v>
       </c>
     </row>
@@ -6150,8 +5632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B106">
-        <v>20210101</v>
+      <c r="B106" s="2">
+        <v>44197</v>
       </c>
       <c r="C106">
         <v>2021</v>
@@ -6190,12 +5672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M106">
+      <c r="L106">
         <v>492313790696.653</v>
       </c>
     </row>
@@ -6205,8 +5682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B107">
-        <v>20210101</v>
+      <c r="B107" s="2">
+        <v>44197</v>
       </c>
       <c r="C107">
         <v>2021</v>
@@ -6245,12 +5722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M107">
+      <c r="L107">
         <v>1562504482.7</v>
       </c>
     </row>
@@ -6260,8 +5732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B108">
-        <v>20210101</v>
+      <c r="B108" s="2">
+        <v>44197</v>
       </c>
       <c r="C108">
         <v>2021</v>
@@ -6300,12 +5772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M108">
+      <c r="L108">
         <v>34719205.288</v>
       </c>
     </row>
@@ -6315,8 +5782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B109">
-        <v>20210101</v>
+      <c r="B109" s="2">
+        <v>44197</v>
       </c>
       <c r="C109">
         <v>2021</v>
@@ -6355,12 +5822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M109">
+      <c r="L109">
         <v>19174845.703</v>
       </c>
     </row>
@@ -6370,8 +5832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B110">
-        <v>20210101</v>
+      <c r="B110" s="2">
+        <v>44197</v>
       </c>
       <c r="C110">
         <v>2021</v>
@@ -6410,12 +5872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L110" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M110">
+      <c r="L110">
         <v>286467258610.596</v>
       </c>
     </row>
@@ -6425,8 +5882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B111">
-        <v>20210101</v>
+      <c r="B111" s="2">
+        <v>44197</v>
       </c>
       <c r="C111">
         <v>2021</v>
@@ -6465,12 +5922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M111">
+      <c r="L111">
         <v>5202221589.634</v>
       </c>
     </row>
@@ -6480,8 +5932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B112">
-        <v>20210101</v>
+      <c r="B112" s="2">
+        <v>44197</v>
       </c>
       <c r="C112">
         <v>2021</v>
@@ -6520,12 +5972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M112">
+      <c r="L112">
         <v>25566160915</v>
       </c>
     </row>
@@ -6535,8 +5982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B113">
-        <v>20210101</v>
+      <c r="B113" s="2">
+        <v>44197</v>
       </c>
       <c r="C113">
         <v>2021</v>
@@ -6575,12 +6022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M113">
+      <c r="L113">
         <v>1951925732.167</v>
       </c>
     </row>
@@ -6590,8 +6032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B114">
-        <v>20210101</v>
+      <c r="B114" s="2">
+        <v>44197</v>
       </c>
       <c r="C114">
         <v>2021</v>
@@ -6630,12 +6072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M114">
+      <c r="L114">
         <v>394813673347.297</v>
       </c>
     </row>
@@ -6645,8 +6082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B115">
-        <v>20210101</v>
+      <c r="B115" s="2">
+        <v>44197</v>
       </c>
       <c r="C115">
         <v>2021</v>
@@ -6685,12 +6122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L115" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M115">
+      <c r="L115">
         <v>457081283281.544</v>
       </c>
     </row>
@@ -6700,8 +6132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B116">
-        <v>20210101</v>
+      <c r="B116" s="2">
+        <v>44197</v>
       </c>
       <c r="C116">
         <v>2021</v>
@@ -6740,12 +6172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L116" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M116">
+      <c r="L116">
         <v>104733320881.922</v>
       </c>
     </row>
@@ -6755,8 +6182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B117">
-        <v>20210101</v>
+      <c r="B117" s="2">
+        <v>44197</v>
       </c>
       <c r="C117">
         <v>2021</v>
@@ -6795,12 +6222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L117" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M117">
+      <c r="L117">
         <v>335792597810</v>
       </c>
     </row>
@@ -6810,8 +6232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B118">
-        <v>20210101</v>
+      <c r="B118" s="2">
+        <v>44197</v>
       </c>
       <c r="C118">
         <v>2021</v>
@@ -6850,12 +6272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L118" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M118">
+      <c r="L118">
         <v>46692128069.11</v>
       </c>
     </row>
@@ -6865,8 +6282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B119">
-        <v>20210101</v>
+      <c r="B119" s="2">
+        <v>44197</v>
       </c>
       <c r="C119">
         <v>2021</v>
@@ -6905,12 +6322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L119" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M119">
+      <c r="L119">
         <v>121321278845.567</v>
       </c>
     </row>
@@ -6920,8 +6332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B120">
-        <v>20210101</v>
+      <c r="B120" s="2">
+        <v>44197</v>
       </c>
       <c r="C120">
         <v>2021</v>
@@ -6960,12 +6372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L120" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M120">
+      <c r="L120">
         <v>6036173160.691</v>
       </c>
     </row>
@@ -6975,8 +6382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B121">
-        <v>20210101</v>
+      <c r="B121" s="2">
+        <v>44197</v>
       </c>
       <c r="C121">
         <v>2021</v>
@@ -7015,12 +6422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L121" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M121">
+      <c r="L121">
         <v>391558519476.67</v>
       </c>
     </row>
@@ -7030,8 +6432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B122">
-        <v>20210101</v>
+      <c r="B122" s="2">
+        <v>44197</v>
       </c>
       <c r="C122">
         <v>2021</v>
@@ -7070,12 +6472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L122" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M122">
+      <c r="L122">
         <v>1513205710.406</v>
       </c>
     </row>
@@ -7085,8 +6482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B123">
-        <v>20210101</v>
+      <c r="B123" s="2">
+        <v>44197</v>
       </c>
       <c r="C123">
         <v>2021</v>
@@ -7125,12 +6522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L123" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M123">
+      <c r="L123">
         <v>2068468810.41</v>
       </c>
     </row>
@@ -7140,8 +6532,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B124">
-        <v>20210101</v>
+      <c r="B124" s="2">
+        <v>44197</v>
       </c>
       <c r="C124">
         <v>2021</v>
@@ -7180,12 +6572,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L124" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M124">
+      <c r="L124">
         <v>189635063199.877</v>
       </c>
     </row>
@@ -7195,8 +6582,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B125">
-        <v>20210101</v>
+      <c r="B125" s="2">
+        <v>44197</v>
       </c>
       <c r="C125">
         <v>2021</v>
@@ -7235,12 +6622,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L125" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M125">
+      <c r="L125">
         <v>379770927042.891</v>
       </c>
     </row>
@@ -7250,8 +6632,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B126">
-        <v>20210101</v>
+      <c r="B126" s="2">
+        <v>44197</v>
       </c>
       <c r="C126">
         <v>2021</v>
@@ -7290,12 +6672,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L126" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M126">
+      <c r="L126">
         <v>1476799996</v>
       </c>
     </row>
@@ -7305,8 +6682,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B127">
-        <v>20210101</v>
+      <c r="B127" s="2">
+        <v>44197</v>
       </c>
       <c r="C127">
         <v>2021</v>
@@ -7345,12 +6722,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L127" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M127">
+      <c r="L127">
         <v>266674796256.73</v>
       </c>
     </row>
@@ -7360,8 +6732,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B128">
-        <v>20210101</v>
+      <c r="B128" s="2">
+        <v>44197</v>
       </c>
       <c r="C128">
         <v>2021</v>
@@ -7400,12 +6772,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L128" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M128">
+      <c r="L128">
         <v>1079792672.912</v>
       </c>
     </row>
@@ -7415,8 +6782,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B129">
-        <v>20210101</v>
+      <c r="B129" s="2">
+        <v>44197</v>
       </c>
       <c r="C129">
         <v>2021</v>
@@ -7455,12 +6822,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L129" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M129">
+      <c r="L129">
         <v>8620228624.916</v>
       </c>
     </row>
@@ -7470,8 +6832,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B130">
-        <v>20210101</v>
+      <c r="B130" s="2">
+        <v>44197</v>
       </c>
       <c r="C130">
         <v>2021</v>
@@ -7510,12 +6872,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L130" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M130">
+      <c r="L130">
         <v>425159796503.562</v>
       </c>
     </row>
@@ -7525,8 +6882,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B131">
-        <v>20210101</v>
+      <c r="B131" s="2">
+        <v>44197</v>
       </c>
       <c r="C131">
         <v>2021</v>
@@ -7565,12 +6922,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L131" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M131">
+      <c r="L131">
         <v>16695198641.544</v>
       </c>
     </row>
@@ -7580,8 +6932,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B132">
-        <v>20210101</v>
+      <c r="B132" s="2">
+        <v>44197</v>
       </c>
       <c r="C132">
         <v>2021</v>
@@ -7620,12 +6972,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L132" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M132">
+      <c r="L132">
         <v>225214458038</v>
       </c>
     </row>
@@ -7635,8 +6982,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B133">
-        <v>20210101</v>
+      <c r="B133" s="2">
+        <v>44197</v>
       </c>
       <c r="C133">
         <v>2021</v>
@@ -7675,12 +7022,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L133" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M133">
+      <c r="L133">
         <v>65870275510.39</v>
       </c>
     </row>
@@ -7690,8 +7032,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B134">
-        <v>20210101</v>
+      <c r="B134" s="2">
+        <v>44197</v>
       </c>
       <c r="C134">
         <v>2021</v>
@@ -7730,12 +7072,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L134" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M134">
+      <c r="L134">
         <v>8186314637.628</v>
       </c>
     </row>
@@ -7745,8 +7082,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B135">
-        <v>20210101</v>
+      <c r="B135" s="2">
+        <v>44197</v>
       </c>
       <c r="C135">
         <v>2021</v>
@@ -7785,12 +7122,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L135" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M135">
+      <c r="L135">
         <v>40701703944.38</v>
       </c>
     </row>
@@ -7800,8 +7132,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B136">
-        <v>20210101</v>
+      <c r="B136" s="2">
+        <v>44197</v>
       </c>
       <c r="C136">
         <v>2021</v>
@@ -7840,12 +7172,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L136" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M136">
+      <c r="L136">
         <v>470547786029.463</v>
       </c>
     </row>
@@ -7855,8 +7182,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B137">
-        <v>20210101</v>
+      <c r="B137" s="2">
+        <v>44197</v>
       </c>
       <c r="C137">
         <v>2021</v>
@@ -7895,12 +7222,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L137" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M137">
+      <c r="L137">
         <v>6390862886.744</v>
       </c>
     </row>
@@ -7910,8 +7232,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B138">
-        <v>20210101</v>
+      <c r="B138" s="2">
+        <v>44197</v>
       </c>
       <c r="C138">
         <v>2021</v>
@@ -7950,12 +7272,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L138" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M138">
+      <c r="L138">
         <v>1753136708106</v>
       </c>
     </row>
@@ -7965,8 +7282,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B139">
-        <v>20210101</v>
+      <c r="B139" s="2">
+        <v>44197</v>
       </c>
       <c r="C139">
         <v>2021</v>
@@ -8005,12 +7322,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L139" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M139">
+      <c r="L139">
         <v>5060027958.95</v>
       </c>
     </row>
@@ -8020,8 +7332,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B140">
-        <v>20210101</v>
+      <c r="B140" s="2">
+        <v>44197</v>
       </c>
       <c r="C140">
         <v>2021</v>
@@ -8060,12 +7372,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L140" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M140">
+      <c r="L140">
         <v>9541020289</v>
       </c>
     </row>
@@ -8075,8 +7382,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B141">
-        <v>20210101</v>
+      <c r="B141" s="2">
+        <v>44197</v>
       </c>
       <c r="C141">
         <v>2021</v>
@@ -8115,12 +7422,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L141" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M141">
+      <c r="L141">
         <v>14092247992.431</v>
       </c>
     </row>
@@ -8130,8 +7432,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B142">
-        <v>20210101</v>
+      <c r="B142" s="2">
+        <v>44197</v>
       </c>
       <c r="C142">
         <v>2021</v>
@@ -8170,12 +7472,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L142" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M142">
+      <c r="L142">
         <v>28836585.461</v>
       </c>
     </row>
@@ -8185,8 +7482,8 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B143">
-        <v>20210101</v>
+      <c r="B143" s="2">
+        <v>44197</v>
       </c>
       <c r="C143">
         <v>2021</v>
@@ -8225,12 +7522,7 @@
           <t>World</t>
         </is>
       </c>
-      <c r="L143" t="inlineStr">
-        <is>
-          <t>All Commodities</t>
-        </is>
-      </c>
-      <c r="M143">
+      <c r="L143">
         <v>10101351858.32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
almost done w/ IMF countries
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021A.xlsx
+++ b/data/comtrade_total_exports_2021A.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4142,16 +4142,16 @@
         <v>52</v>
       </c>
       <c r="E76">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>MYS</t>
+          <t>MWI</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Malawi</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4173,7 +4173,7 @@
         </is>
       </c>
       <c r="L76">
-        <v>299230434394.232</v>
+        <v>1009460778.534</v>
       </c>
     </row>
     <row r="77">
@@ -4192,16 +4192,16 @@
         <v>52</v>
       </c>
       <c r="E77">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>MDV</t>
+          <t>MYS</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -4223,7 +4223,7 @@
         </is>
       </c>
       <c r="L77">
-        <v>151293266.49</v>
+        <v>299230434394.232</v>
       </c>
     </row>
     <row r="78">
@@ -4242,16 +4242,16 @@
         <v>52</v>
       </c>
       <c r="E78">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>MLT</t>
+          <t>MDV</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Maldives</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4273,7 +4273,7 @@
         </is>
       </c>
       <c r="L78">
-        <v>3200429629.51</v>
+        <v>151293266.49</v>
       </c>
     </row>
     <row r="79">
@@ -4292,16 +4292,16 @@
         <v>52</v>
       </c>
       <c r="E79">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>MRT</t>
+          <t>MLT</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Mauritania</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -4323,7 +4323,7 @@
         </is>
       </c>
       <c r="L79">
-        <v>3266988807.55</v>
+        <v>3200429629.51</v>
       </c>
     </row>
     <row r="80">
@@ -4342,16 +4342,16 @@
         <v>52</v>
       </c>
       <c r="E80">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>MUS</t>
+          <t>MRT</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Mauritius</t>
+          <t>Mauritania</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -4373,7 +4373,7 @@
         </is>
       </c>
       <c r="L80">
-        <v>1671760288.267</v>
+        <v>3266988807.55</v>
       </c>
     </row>
     <row r="81">
@@ -4392,16 +4392,16 @@
         <v>52</v>
       </c>
       <c r="E81">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MUS</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Mauritius</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -4423,7 +4423,7 @@
         </is>
       </c>
       <c r="L81">
-        <v>494595503435</v>
+        <v>1671760288.267</v>
       </c>
     </row>
     <row r="82">
@@ -4442,16 +4442,16 @@
         <v>52</v>
       </c>
       <c r="E82">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>S19</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Other Asia, nes</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -4473,7 +4473,7 @@
         </is>
       </c>
       <c r="L82">
-        <v>447656546120.094</v>
+        <v>494595503435</v>
       </c>
     </row>
     <row r="83">
@@ -4492,16 +4492,16 @@
         <v>52</v>
       </c>
       <c r="E83">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>MNG</t>
+          <t>S19</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Other Asia, nes</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -4523,7 +4523,7 @@
         </is>
       </c>
       <c r="L83">
-        <v>9241123149.940001</v>
+        <v>447656546120.094</v>
       </c>
     </row>
     <row r="84">
@@ -4542,16 +4542,16 @@
         <v>52</v>
       </c>
       <c r="E84">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>MDA</t>
+          <t>MNG</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Rep. of Moldova</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -4573,7 +4573,7 @@
         </is>
       </c>
       <c r="L84">
-        <v>3144504817</v>
+        <v>9241123149.940001</v>
       </c>
     </row>
     <row r="85">
@@ -4592,16 +4592,16 @@
         <v>52</v>
       </c>
       <c r="E85">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>MNE</t>
+          <t>MDA</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Rep. of Moldova</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -4623,7 +4623,7 @@
         </is>
       </c>
       <c r="L85">
-        <v>515916303.811</v>
+        <v>3144504817</v>
       </c>
     </row>
     <row r="86">
@@ -4642,16 +4642,16 @@
         <v>52</v>
       </c>
       <c r="E86">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>MAR</t>
+          <t>MNE</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -4673,7 +4673,7 @@
         </is>
       </c>
       <c r="L86">
-        <v>36585224951.204</v>
+        <v>515916303.811</v>
       </c>
     </row>
     <row r="87">
@@ -4692,16 +4692,16 @@
         <v>52</v>
       </c>
       <c r="E87">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>MOZ</t>
+          <t>MAR</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -4723,7 +4723,7 @@
         </is>
       </c>
       <c r="L87">
-        <v>5111685900.99</v>
+        <v>36585224951.204</v>
       </c>
     </row>
     <row r="88">
@@ -4742,16 +4742,16 @@
         <v>52</v>
       </c>
       <c r="E88">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>OMN</t>
+          <t>MOZ</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Oman</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -4773,7 +4773,7 @@
         </is>
       </c>
       <c r="L88">
-        <v>44590926520.592</v>
+        <v>5111685900.99</v>
       </c>
     </row>
     <row r="89">
@@ -4792,16 +4792,16 @@
         <v>52</v>
       </c>
       <c r="E89">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>NPL</t>
+          <t>OMN</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Oman</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -4823,7 +4823,7 @@
         </is>
       </c>
       <c r="L89">
-        <v>1665727794.55</v>
+        <v>44590926520.592</v>
       </c>
     </row>
     <row r="90">
@@ -4842,16 +4842,16 @@
         <v>52</v>
       </c>
       <c r="E90">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>NLD</t>
+          <t>NPL</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -4873,7 +4873,7 @@
         </is>
       </c>
       <c r="L90">
-        <v>696873257184.973</v>
+        <v>1665727794.55</v>
       </c>
     </row>
     <row r="91">
@@ -4892,16 +4892,16 @@
         <v>52</v>
       </c>
       <c r="E91">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>ABW</t>
+          <t>NLD</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -4923,7 +4923,7 @@
         </is>
       </c>
       <c r="L91">
-        <v>88347007.693</v>
+        <v>696873257184.973</v>
       </c>
     </row>
     <row r="92">
@@ -4942,16 +4942,16 @@
         <v>52</v>
       </c>
       <c r="E92">
-        <v>554</v>
+        <v>533</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>NZL</t>
+          <t>ABW</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -4973,7 +4973,7 @@
         </is>
       </c>
       <c r="L92">
-        <v>44325287820.466</v>
+        <v>88347007.693</v>
       </c>
     </row>
     <row r="93">
@@ -4992,16 +4992,16 @@
         <v>52</v>
       </c>
       <c r="E93">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>NIC</t>
+          <t>NZL</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -5023,7 +5023,7 @@
         </is>
       </c>
       <c r="L93">
-        <v>6494984866.92</v>
+        <v>44325287820.466</v>
       </c>
     </row>
     <row r="94">
@@ -5042,16 +5042,16 @@
         <v>52</v>
       </c>
       <c r="E94">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>NER</t>
+          <t>NIC</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Niger</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -5073,7 +5073,7 @@
         </is>
       </c>
       <c r="L94">
-        <v>506672560.08</v>
+        <v>6494984866.92</v>
       </c>
     </row>
     <row r="95">
@@ -5092,16 +5092,16 @@
         <v>52</v>
       </c>
       <c r="E95">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>NGA</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -5123,7 +5123,7 @@
         </is>
       </c>
       <c r="L95">
-        <v>47231712930.364</v>
+        <v>506672560.08</v>
       </c>
     </row>
     <row r="96">
@@ -5142,16 +5142,16 @@
         <v>52</v>
       </c>
       <c r="E96">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>NOR</t>
+          <t>NGA</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5173,7 +5173,7 @@
         </is>
       </c>
       <c r="L96">
-        <v>161686747944.171</v>
+        <v>47231712930.364</v>
       </c>
     </row>
     <row r="97">
@@ -5192,16 +5192,16 @@
         <v>52</v>
       </c>
       <c r="E97">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>PAK</t>
+          <t>NOR</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -5223,7 +5223,7 @@
         </is>
       </c>
       <c r="L97">
-        <v>28795179085.962</v>
+        <v>161686747944.171</v>
       </c>
     </row>
     <row r="98">
@@ -5242,16 +5242,16 @@
         <v>52</v>
       </c>
       <c r="E98">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>PAK</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -5273,7 +5273,7 @@
         </is>
       </c>
       <c r="L98">
-        <v>3781922651</v>
+        <v>28795179085.962</v>
       </c>
     </row>
     <row r="99">
@@ -5292,16 +5292,16 @@
         <v>52</v>
       </c>
       <c r="E99">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>PRY</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -5323,7 +5323,7 @@
         </is>
       </c>
       <c r="L99">
-        <v>10570969868</v>
+        <v>3781922651</v>
       </c>
     </row>
     <row r="100">
@@ -5342,16 +5342,16 @@
         <v>52</v>
       </c>
       <c r="E100">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>PRY</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -5373,7 +5373,7 @@
         </is>
       </c>
       <c r="L100">
-        <v>56260115202.756</v>
+        <v>10570969868</v>
       </c>
     </row>
     <row r="101">
@@ -5392,16 +5392,16 @@
         <v>52</v>
       </c>
       <c r="E101">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -5423,7 +5423,7 @@
         </is>
       </c>
       <c r="L101">
-        <v>74619528755</v>
+        <v>56260115202.756</v>
       </c>
     </row>
     <row r="102">
@@ -5442,16 +5442,16 @@
         <v>52</v>
       </c>
       <c r="E102">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>POL</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -5473,7 +5473,7 @@
         </is>
       </c>
       <c r="L102">
-        <v>317832124942</v>
+        <v>74619528755</v>
       </c>
     </row>
     <row r="103">
@@ -5492,16 +5492,16 @@
         <v>52</v>
       </c>
       <c r="E103">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>POL</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -5523,7 +5523,7 @@
         </is>
       </c>
       <c r="L103">
-        <v>75242766894.064</v>
+        <v>317832124942</v>
       </c>
     </row>
     <row r="104">
@@ -5542,16 +5542,16 @@
         <v>52</v>
       </c>
       <c r="E104">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>QAT</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Qatar</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -5573,7 +5573,7 @@
         </is>
       </c>
       <c r="L104">
-        <v>87203291188.87</v>
+        <v>75242766894.064</v>
       </c>
     </row>
     <row r="105">
@@ -5592,16 +5592,16 @@
         <v>52</v>
       </c>
       <c r="E105">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>ROU</t>
+          <t>QAT</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Qatar</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -5623,7 +5623,7 @@
         </is>
       </c>
       <c r="L105">
-        <v>88389728970.91</v>
+        <v>87203291188.87</v>
       </c>
     </row>
     <row r="106">
@@ -5642,16 +5642,16 @@
         <v>52</v>
       </c>
       <c r="E106">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>ROU</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Russian Federation</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -5673,7 +5673,7 @@
         </is>
       </c>
       <c r="L106">
-        <v>492313790696.653</v>
+        <v>88389728970.91</v>
       </c>
     </row>
     <row r="107">
@@ -5692,16 +5692,16 @@
         <v>52</v>
       </c>
       <c r="E107">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -5723,7 +5723,7 @@
         </is>
       </c>
       <c r="L107">
-        <v>1562504482.7</v>
+        <v>492313790696.653</v>
       </c>
     </row>
     <row r="108">
@@ -5742,16 +5742,16 @@
         <v>52</v>
       </c>
       <c r="E108">
-        <v>670</v>
+        <v>646</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>VCT</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Saint Vincent and the Grenadines</t>
+          <t>Rwanda</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -5773,7 +5773,7 @@
         </is>
       </c>
       <c r="L108">
-        <v>34719205.288</v>
+        <v>1562504482.7</v>
       </c>
     </row>
     <row r="109">
@@ -5792,16 +5792,16 @@
         <v>52</v>
       </c>
       <c r="E109">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>STP</t>
+          <t>VCT</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Sao Tome and Principe</t>
+          <t>Saint Vincent and the Grenadines</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -5823,7 +5823,7 @@
         </is>
       </c>
       <c r="L109">
-        <v>19174845.703</v>
+        <v>34719205.288</v>
       </c>
     </row>
     <row r="110">
@@ -5842,16 +5842,16 @@
         <v>52</v>
       </c>
       <c r="E110">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>SAU</t>
+          <t>STP</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Sao Tome and Principe</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -5873,7 +5873,7 @@
         </is>
       </c>
       <c r="L110">
-        <v>286467258610.596</v>
+        <v>19174845.703</v>
       </c>
     </row>
     <row r="111">
@@ -5892,16 +5892,16 @@
         <v>52</v>
       </c>
       <c r="E111">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>SEN</t>
+          <t>SAU</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Senegal</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -5923,7 +5923,7 @@
         </is>
       </c>
       <c r="L111">
-        <v>5202221589.634</v>
+        <v>286467258610.596</v>
       </c>
     </row>
     <row r="112">
@@ -5942,16 +5942,16 @@
         <v>52</v>
       </c>
       <c r="E112">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>SEN</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Senegal</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -5973,7 +5973,7 @@
         </is>
       </c>
       <c r="L112">
-        <v>25566160915</v>
+        <v>5202221589.634</v>
       </c>
     </row>
     <row r="113">
@@ -5992,16 +5992,16 @@
         <v>52</v>
       </c>
       <c r="E113">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>SYC</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Seychelles</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -6023,7 +6023,7 @@
         </is>
       </c>
       <c r="L113">
-        <v>1951925732.167</v>
+        <v>25566160915</v>
       </c>
     </row>
     <row r="114">
@@ -6042,16 +6042,16 @@
         <v>52</v>
       </c>
       <c r="E114">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>SYC</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Seychelles</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -6073,7 +6073,7 @@
         </is>
       </c>
       <c r="L114">
-        <v>394813673347.297</v>
+        <v>1951925732.167</v>
       </c>
     </row>
     <row r="115">
@@ -6092,16 +6092,16 @@
         <v>52</v>
       </c>
       <c r="E115">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>SGP</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>India</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -6123,7 +6123,7 @@
         </is>
       </c>
       <c r="L115">
-        <v>457081283281.544</v>
+        <v>394813673347.297</v>
       </c>
     </row>
     <row r="116">
@@ -6142,16 +6142,16 @@
         <v>52</v>
       </c>
       <c r="E116">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>SVK</t>
+          <t>SGP</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -6173,7 +6173,7 @@
         </is>
       </c>
       <c r="L116">
-        <v>104733320881.922</v>
+        <v>457081283281.544</v>
       </c>
     </row>
     <row r="117">
@@ -6192,16 +6192,16 @@
         <v>52</v>
       </c>
       <c r="E117">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>VNM</t>
+          <t>SVK</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Viet Nam</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -6223,7 +6223,7 @@
         </is>
       </c>
       <c r="L117">
-        <v>335792597810</v>
+        <v>104733320881.922</v>
       </c>
     </row>
     <row r="118">
@@ -6242,16 +6242,16 @@
         <v>52</v>
       </c>
       <c r="E118">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>VNM</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Viet Nam</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -6273,7 +6273,7 @@
         </is>
       </c>
       <c r="L118">
-        <v>46692128069.11</v>
+        <v>335792597810</v>
       </c>
     </row>
     <row r="119">
@@ -6292,16 +6292,16 @@
         <v>52</v>
       </c>
       <c r="E119">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>ZAF</t>
+          <t>SVN</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -6323,7 +6323,7 @@
         </is>
       </c>
       <c r="L119">
-        <v>121321278845.567</v>
+        <v>46692128069.11</v>
       </c>
     </row>
     <row r="120">
@@ -6342,16 +6342,16 @@
         <v>52</v>
       </c>
       <c r="E120">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>ZWE</t>
+          <t>ZAF</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -6373,7 +6373,7 @@
         </is>
       </c>
       <c r="L120">
-        <v>6036173160.691</v>
+        <v>121321278845.567</v>
       </c>
     </row>
     <row r="121">
@@ -6392,16 +6392,16 @@
         <v>52</v>
       </c>
       <c r="E121">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>ESP</t>
+          <t>ZWE</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -6423,7 +6423,7 @@
         </is>
       </c>
       <c r="L121">
-        <v>391558519476.67</v>
+        <v>6036173160.691</v>
       </c>
     </row>
     <row r="122">
@@ -6442,16 +6442,16 @@
         <v>52</v>
       </c>
       <c r="E122">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>SUR</t>
+          <t>ESP</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -6473,7 +6473,7 @@
         </is>
       </c>
       <c r="L122">
-        <v>1513205710.406</v>
+        <v>391558519476.67</v>
       </c>
     </row>
     <row r="123">
@@ -6492,16 +6492,16 @@
         <v>52</v>
       </c>
       <c r="E123">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>SWZ</t>
+          <t>SUR</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Suriname</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -6523,7 +6523,7 @@
         </is>
       </c>
       <c r="L123">
-        <v>2068468810.41</v>
+        <v>1513205710.406</v>
       </c>
     </row>
     <row r="124">
@@ -6542,16 +6542,16 @@
         <v>52</v>
       </c>
       <c r="E124">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>SWE</t>
+          <t>SWZ</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Eswatini</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -6573,7 +6573,7 @@
         </is>
       </c>
       <c r="L124">
-        <v>189635063199.877</v>
+        <v>2068468810.41</v>
       </c>
     </row>
     <row r="125">
@@ -6592,16 +6592,16 @@
         <v>52</v>
       </c>
       <c r="E125">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>CHE</t>
+          <t>SWE</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -6623,7 +6623,7 @@
         </is>
       </c>
       <c r="L125">
-        <v>379770927042.891</v>
+        <v>189635063199.877</v>
       </c>
     </row>
     <row r="126">
@@ -6642,16 +6642,16 @@
         <v>52</v>
       </c>
       <c r="E126">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>CHE</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -6673,7 +6673,7 @@
         </is>
       </c>
       <c r="L126">
-        <v>1476799996</v>
+        <v>379770927042.891</v>
       </c>
     </row>
     <row r="127">
@@ -6692,16 +6692,16 @@
         <v>52</v>
       </c>
       <c r="E127">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>THA</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Tajikistan</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -6723,7 +6723,7 @@
         </is>
       </c>
       <c r="L127">
-        <v>266674796256.73</v>
+        <v>1476799996</v>
       </c>
     </row>
     <row r="128">
@@ -6742,16 +6742,16 @@
         <v>52</v>
       </c>
       <c r="E128">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>TGO</t>
+          <t>THA</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -6773,7 +6773,7 @@
         </is>
       </c>
       <c r="L128">
-        <v>1079792672.912</v>
+        <v>266674796256.73</v>
       </c>
     </row>
     <row r="129">
@@ -6792,16 +6792,16 @@
         <v>52</v>
       </c>
       <c r="E129">
-        <v>780</v>
+        <v>768</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>TTO</t>
+          <t>TGO</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Togo</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -6823,7 +6823,7 @@
         </is>
       </c>
       <c r="L129">
-        <v>8620228624.916</v>
+        <v>1079792672.912</v>
       </c>
     </row>
     <row r="130">
@@ -6842,16 +6842,16 @@
         <v>52</v>
       </c>
       <c r="E130">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>ARE</t>
+          <t>TTO</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -6873,7 +6873,7 @@
         </is>
       </c>
       <c r="L130">
-        <v>425159796503.562</v>
+        <v>8620228624.916</v>
       </c>
     </row>
     <row r="131">
@@ -6892,16 +6892,16 @@
         <v>52</v>
       </c>
       <c r="E131">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>ARE</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -6923,7 +6923,7 @@
         </is>
       </c>
       <c r="L131">
-        <v>16695198641.544</v>
+        <v>425159796503.562</v>
       </c>
     </row>
     <row r="132">
@@ -6942,16 +6942,16 @@
         <v>52</v>
       </c>
       <c r="E132">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>TUR</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Türkiye</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -6973,7 +6973,7 @@
         </is>
       </c>
       <c r="L132">
-        <v>225214458038</v>
+        <v>16695198641.544</v>
       </c>
     </row>
     <row r="133">
@@ -6992,16 +6992,16 @@
         <v>52</v>
       </c>
       <c r="E133">
-        <v>804</v>
+        <v>792</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TUR</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Türkiye</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -7023,7 +7023,7 @@
         </is>
       </c>
       <c r="L133">
-        <v>65870275510.39</v>
+        <v>225214458038</v>
       </c>
     </row>
     <row r="134">
@@ -7042,16 +7042,16 @@
         <v>52</v>
       </c>
       <c r="E134">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>MKD</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -7073,7 +7073,7 @@
         </is>
       </c>
       <c r="L134">
-        <v>8186314637.628</v>
+        <v>65870275510.39</v>
       </c>
     </row>
     <row r="135">
@@ -7092,16 +7092,16 @@
         <v>52</v>
       </c>
       <c r="E135">
-        <v>818</v>
+        <v>807</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>EGY</t>
+          <t>MKD</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
@@ -7123,7 +7123,7 @@
         </is>
       </c>
       <c r="L135">
-        <v>40701703944.38</v>
+        <v>8186314637.628</v>
       </c>
     </row>
     <row r="136">
@@ -7142,16 +7142,16 @@
         <v>52</v>
       </c>
       <c r="E136">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>GBR</t>
+          <t>EGY</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -7173,7 +7173,7 @@
         </is>
       </c>
       <c r="L136">
-        <v>470547786029.463</v>
+        <v>40701703944.38</v>
       </c>
     </row>
     <row r="137">
@@ -7192,16 +7192,16 @@
         <v>52</v>
       </c>
       <c r="E137">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>TZA</t>
+          <t>GBR</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>United Rep. of Tanzania</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -7223,7 +7223,7 @@
         </is>
       </c>
       <c r="L137">
-        <v>6390862886.744</v>
+        <v>470547786029.463</v>
       </c>
     </row>
     <row r="138">
@@ -7242,16 +7242,16 @@
         <v>52</v>
       </c>
       <c r="E138">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>TZA</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United Rep. of Tanzania</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -7273,7 +7273,7 @@
         </is>
       </c>
       <c r="L138">
-        <v>1753136708106</v>
+        <v>6390862886.744</v>
       </c>
     </row>
     <row r="139">
@@ -7292,16 +7292,16 @@
         <v>52</v>
       </c>
       <c r="E139">
-        <v>854</v>
+        <v>842</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>BFA</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Burkina Faso</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -7323,7 +7323,7 @@
         </is>
       </c>
       <c r="L139">
-        <v>5060027958.95</v>
+        <v>1753136708106</v>
       </c>
     </row>
     <row r="140">
@@ -7342,16 +7342,16 @@
         <v>52</v>
       </c>
       <c r="E140">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>URY</t>
+          <t>BFA</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Burkina Faso</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -7373,7 +7373,7 @@
         </is>
       </c>
       <c r="L140">
-        <v>9541020289</v>
+        <v>5060027958.95</v>
       </c>
     </row>
     <row r="141">
@@ -7392,16 +7392,16 @@
         <v>52</v>
       </c>
       <c r="E141">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>URY</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -7423,7 +7423,7 @@
         </is>
       </c>
       <c r="L141">
-        <v>14092247992.431</v>
+        <v>9541020289</v>
       </c>
     </row>
     <row r="142">
@@ -7442,16 +7442,16 @@
         <v>52</v>
       </c>
       <c r="E142">
-        <v>882</v>
+        <v>860</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Samoa</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -7473,7 +7473,7 @@
         </is>
       </c>
       <c r="L142">
-        <v>28836585.461</v>
+        <v>14092247992.431</v>
       </c>
     </row>
     <row r="143">
@@ -7492,37 +7492,87 @@
         <v>52</v>
       </c>
       <c r="E143">
+        <v>882</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>WSM</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Export</t>
+        </is>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>W00</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+      <c r="L143">
+        <v>28836585.461</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B144" s="2">
+        <v>44197</v>
+      </c>
+      <c r="C144">
+        <v>2021</v>
+      </c>
+      <c r="D144">
+        <v>52</v>
+      </c>
+      <c r="E144">
         <v>894</v>
       </c>
-      <c r="F143" t="inlineStr">
+      <c r="F144" t="inlineStr">
         <is>
           <t>ZMB</t>
         </is>
       </c>
-      <c r="G143" t="inlineStr">
+      <c r="G144" t="inlineStr">
         <is>
           <t>Zambia</t>
         </is>
       </c>
-      <c r="H143" t="inlineStr">
-        <is>
-          <t>Export</t>
-        </is>
-      </c>
-      <c r="I143">
-        <v>0</v>
-      </c>
-      <c r="J143" t="inlineStr">
-        <is>
-          <t>W00</t>
-        </is>
-      </c>
-      <c r="K143" t="inlineStr">
-        <is>
-          <t>World</t>
-        </is>
-      </c>
-      <c r="L143">
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Export</t>
+        </is>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>W00</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+      <c r="L144">
         <v>10101351858.32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on date issues
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021A.xlsx
+++ b/data/comtrade_total_exports_2021A.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -769,11 +769,11 @@
         <v>44197</v>
       </c>
       <c r="B23">
-        <v>17082261.232</v>
+        <v>501538854874.334</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Cayman Isds</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -787,11 +787,11 @@
         <v>44197</v>
       </c>
       <c r="B24">
-        <v>13331248583.322</v>
+        <v>17082261.232</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Sri Lanka</t>
+          <t>Cayman Isds</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -805,11 +805,11 @@
         <v>44197</v>
       </c>
       <c r="B25">
-        <v>94676809206.28101</v>
+        <v>13331248583.322</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Sri Lanka</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -823,11 +823,11 @@
         <v>44197</v>
       </c>
       <c r="B26">
-        <v>3362301613439</v>
+        <v>94676809206.28101</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -841,11 +841,11 @@
         <v>44197</v>
       </c>
       <c r="B27">
-        <v>41389989047.59</v>
+        <v>3362301613439</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>China</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -859,11 +859,11 @@
         <v>44197</v>
       </c>
       <c r="B28">
-        <v>34994132.52</v>
+        <v>41389989047.59</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Comoros</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -877,11 +877,11 @@
         <v>44197</v>
       </c>
       <c r="B29">
-        <v>2362230161.01</v>
+        <v>34994132.52</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Congo</t>
+          <t>Comoros</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -895,11 +895,11 @@
         <v>44197</v>
       </c>
       <c r="B30">
-        <v>24124651297.35</v>
+        <v>2362230161.01</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dem. Rep. of the Congo</t>
+          <t>Congo</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -913,11 +913,11 @@
         <v>44197</v>
       </c>
       <c r="B31">
-        <v>14345395565.22</v>
+        <v>24124651297.35</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Dem. Rep. of the Congo</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -931,11 +931,11 @@
         <v>44197</v>
       </c>
       <c r="B32">
-        <v>21827948964</v>
+        <v>14345395565.22</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -949,11 +949,11 @@
         <v>44197</v>
       </c>
       <c r="B33">
-        <v>3989812264.347</v>
+        <v>21827948964</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -967,11 +967,11 @@
         <v>44197</v>
       </c>
       <c r="B34">
-        <v>227168411022</v>
+        <v>3989812264.347</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Czechia</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -985,11 +985,11 @@
         <v>44197</v>
       </c>
       <c r="B35">
-        <v>1023522023.899</v>
+        <v>227168411022</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Benin</t>
+          <t>Czechia</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1003,11 +1003,11 @@
         <v>44197</v>
       </c>
       <c r="B36">
-        <v>125014614347.861</v>
+        <v>1023522023.899</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Benin</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1021,11 +1021,11 @@
         <v>44197</v>
       </c>
       <c r="B37">
-        <v>11725013719.98</v>
+        <v>125014614347.861</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Dominican Rep.</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1039,11 +1039,11 @@
         <v>44197</v>
       </c>
       <c r="B38">
-        <v>26699199844.372</v>
+        <v>11725013719.98</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Dominican Rep.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1057,11 +1057,11 @@
         <v>44197</v>
       </c>
       <c r="B39">
-        <v>6394888915.91</v>
+        <v>26699199844.372</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1075,11 +1075,11 @@
         <v>44197</v>
       </c>
       <c r="B40">
-        <v>3057628826.59</v>
+        <v>6394888915.91</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ethiopia</t>
+          <t>El Salvador</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1093,11 +1093,11 @@
         <v>44197</v>
       </c>
       <c r="B41">
-        <v>22282223314.05</v>
+        <v>3057628826.59</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1111,11 +1111,11 @@
         <v>44197</v>
       </c>
       <c r="B42">
-        <v>815335653.153</v>
+        <v>22282223314.05</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Fiji</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1129,11 +1129,11 @@
         <v>44197</v>
       </c>
       <c r="B43">
-        <v>81500265209.30499</v>
+        <v>815335653.153</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Fiji</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1147,11 +1147,11 @@
         <v>44197</v>
       </c>
       <c r="B44">
-        <v>585148036598.849</v>
+        <v>81500265209.30499</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1165,11 +1165,11 @@
         <v>44197</v>
       </c>
       <c r="B45">
-        <v>4242653017.17</v>
+        <v>585148036598.849</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1183,11 +1183,11 @@
         <v>44197</v>
       </c>
       <c r="B46">
-        <v>26401460.44</v>
+        <v>4242653017.17</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Gambia</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1201,11 +1201,11 @@
         <v>44197</v>
       </c>
       <c r="B47">
-        <v>1357640029.17</v>
+        <v>26401460.44</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>State of Palestine</t>
+          <t>Gambia</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1219,11 +1219,11 @@
         <v>44197</v>
       </c>
       <c r="B48">
-        <v>1635599573787.609</v>
+        <v>1357640029.17</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>State of Palestine</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1237,11 +1237,11 @@
         <v>44197</v>
       </c>
       <c r="B49">
-        <v>47244277316.697</v>
+        <v>1635599573787.609</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1255,11 +1255,11 @@
         <v>44197</v>
       </c>
       <c r="B50">
-        <v>35163394.409</v>
+        <v>47244277316.697</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Grenada</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1273,11 +1273,11 @@
         <v>44197</v>
       </c>
       <c r="B51">
-        <v>13735599195</v>
+        <v>35163394.409</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Grenada</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1291,11 +1291,11 @@
         <v>44197</v>
       </c>
       <c r="B52">
-        <v>4257250461.689</v>
+        <v>13735599195</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1309,11 +1309,11 @@
         <v>44197</v>
       </c>
       <c r="B53">
-        <v>4975948988.14</v>
+        <v>4257250461.689</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Guyana</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1327,11 +1327,11 @@
         <v>44197</v>
       </c>
       <c r="B54">
-        <v>670926079457.053</v>
+        <v>4975948988.14</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>China, Hong Kong SAR</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1345,11 +1345,11 @@
         <v>44197</v>
       </c>
       <c r="B55">
-        <v>141157091681</v>
+        <v>670926079457.053</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>China, Hong Kong SAR</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1363,11 +1363,11 @@
         <v>44197</v>
       </c>
       <c r="B56">
-        <v>5973742650.46</v>
+        <v>141157091681</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1381,11 +1381,11 @@
         <v>44197</v>
       </c>
       <c r="B57">
-        <v>231522458128.8</v>
+        <v>5973742650.46</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1399,11 +1399,11 @@
         <v>44197</v>
       </c>
       <c r="B58">
-        <v>195997875900.844</v>
+        <v>231522458128.8</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1417,11 +1417,11 @@
         <v>44197</v>
       </c>
       <c r="B59">
-        <v>60159734000</v>
+        <v>195997875900.844</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1435,11 +1435,11 @@
         <v>44197</v>
       </c>
       <c r="B60">
-        <v>615910260060.774</v>
+        <v>60159734000</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1453,11 +1453,11 @@
         <v>44197</v>
       </c>
       <c r="B61">
-        <v>1440530765.28</v>
+        <v>615910260060.774</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1471,11 +1471,11 @@
         <v>44197</v>
       </c>
       <c r="B62">
-        <v>757066261248.9709</v>
+        <v>1440530765.28</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1489,11 +1489,11 @@
         <v>44197</v>
       </c>
       <c r="B63">
-        <v>9356550020.493999</v>
+        <v>757066261248.9709</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1507,11 +1507,11 @@
         <v>44197</v>
       </c>
       <c r="B64">
-        <v>6751366221.034</v>
+        <v>9356550020.493999</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Jordan</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1525,11 +1525,11 @@
         <v>44197</v>
       </c>
       <c r="B65">
-        <v>644411147014</v>
+        <v>6751366221.034</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Rep. of Korea</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1543,11 +1543,11 @@
         <v>44197</v>
       </c>
       <c r="B66">
-        <v>63129693952</v>
+        <v>644411147014</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Kuwait</t>
+          <t>Rep. of Korea</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1561,11 +1561,11 @@
         <v>44197</v>
       </c>
       <c r="B67">
-        <v>2752163636</v>
+        <v>63129693952</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>Kuwait</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1579,11 +1579,11 @@
         <v>44197</v>
       </c>
       <c r="B68">
-        <v>7164605459.07</v>
+        <v>2752163636</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Lao People's Dem. Rep.</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1597,11 +1597,11 @@
         <v>44197</v>
       </c>
       <c r="B69">
-        <v>4229976738</v>
+        <v>7164605459.07</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Lao People's Dem. Rep.</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1615,11 +1615,11 @@
         <v>44197</v>
       </c>
       <c r="B70">
-        <v>948535188.45</v>
+        <v>4229976738</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Lesotho</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1633,11 +1633,11 @@
         <v>44197</v>
       </c>
       <c r="B71">
-        <v>19458821916.273</v>
+        <v>948535188.45</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Lesotho</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1651,11 +1651,11 @@
         <v>44197</v>
       </c>
       <c r="B72">
-        <v>40698383278.78</v>
+        <v>19458821916.273</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1669,11 +1669,11 @@
         <v>44197</v>
       </c>
       <c r="B73">
-        <v>16247126542.139</v>
+        <v>40698383278.78</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1687,11 +1687,11 @@
         <v>44197</v>
       </c>
       <c r="B74">
-        <v>1392424900.553</v>
+        <v>16247126542.139</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>China, Macao SAR</t>
+          <t>Luxembourg</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1705,11 +1705,11 @@
         <v>44197</v>
       </c>
       <c r="B75">
-        <v>2788376340.521</v>
+        <v>1392424900.553</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>China, Macao SAR</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1723,11 +1723,11 @@
         <v>44197</v>
       </c>
       <c r="B76">
-        <v>1009460778.534</v>
+        <v>2788376340.521</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Malawi</t>
+          <t>Madagascar</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1741,11 +1741,11 @@
         <v>44197</v>
       </c>
       <c r="B77">
-        <v>299230434394.232</v>
+        <v>1009460778.534</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Malawi</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1759,11 +1759,11 @@
         <v>44197</v>
       </c>
       <c r="B78">
-        <v>151293266.49</v>
+        <v>299230434394.232</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -1777,11 +1777,11 @@
         <v>44197</v>
       </c>
       <c r="B79">
-        <v>3066831630.829</v>
+        <v>151293266.49</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Maldives</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -1795,11 +1795,11 @@
         <v>44197</v>
       </c>
       <c r="B80">
-        <v>3266988807.55</v>
+        <v>3066831630.829</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Mauritania</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -1813,11 +1813,11 @@
         <v>44197</v>
       </c>
       <c r="B81">
-        <v>1671760288.267</v>
+        <v>3266988807.55</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Mauritius</t>
+          <t>Mauritania</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -1831,11 +1831,11 @@
         <v>44197</v>
       </c>
       <c r="B82">
-        <v>494595503435</v>
+        <v>1671760288.267</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Mauritius</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -1849,11 +1849,11 @@
         <v>44197</v>
       </c>
       <c r="B83">
-        <v>447656546120.094</v>
+        <v>494595503435</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Other Asia, nes</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -1867,11 +1867,11 @@
         <v>44197</v>
       </c>
       <c r="B84">
-        <v>9241123149.940001</v>
+        <v>447656546120.094</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Other Asia, nes</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -1885,11 +1885,11 @@
         <v>44197</v>
       </c>
       <c r="B85">
-        <v>3144504817</v>
+        <v>9241123149.940001</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Rep. of Moldova</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -1903,11 +1903,11 @@
         <v>44197</v>
       </c>
       <c r="B86">
-        <v>515916303.811</v>
+        <v>3144504817</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Rep. of Moldova</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -1921,11 +1921,11 @@
         <v>44197</v>
       </c>
       <c r="B87">
-        <v>36585224951.204</v>
+        <v>515916303.811</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -1939,11 +1939,11 @@
         <v>44197</v>
       </c>
       <c r="B88">
-        <v>5111685900.99</v>
+        <v>36585224951.204</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -1957,11 +1957,11 @@
         <v>44197</v>
       </c>
       <c r="B89">
-        <v>44590926520.592</v>
+        <v>5111685900.99</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Oman</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -1975,11 +1975,11 @@
         <v>44197</v>
       </c>
       <c r="B90">
-        <v>1665727794.55</v>
+        <v>44590926520.592</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Oman</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -1993,11 +1993,11 @@
         <v>44197</v>
       </c>
       <c r="B91">
-        <v>696873257184.973</v>
+        <v>1665727794.55</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2011,11 +2011,11 @@
         <v>44197</v>
       </c>
       <c r="B92">
-        <v>88347007.693</v>
+        <v>696873257184.973</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2029,11 +2029,11 @@
         <v>44197</v>
       </c>
       <c r="B93">
-        <v>44325287820.466</v>
+        <v>88347007.693</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2047,11 +2047,11 @@
         <v>44197</v>
       </c>
       <c r="B94">
-        <v>6494984866.92</v>
+        <v>44325287820.466</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2065,11 +2065,11 @@
         <v>44197</v>
       </c>
       <c r="B95">
-        <v>506672560.08</v>
+        <v>6494984866.92</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Niger</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2083,11 +2083,11 @@
         <v>44197</v>
       </c>
       <c r="B96">
-        <v>47231712930.364</v>
+        <v>506672560.08</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2101,11 +2101,11 @@
         <v>44197</v>
       </c>
       <c r="B97">
-        <v>174513974109.642</v>
+        <v>47231712930.364</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2119,11 +2119,11 @@
         <v>44197</v>
       </c>
       <c r="B98">
-        <v>28795179085.962</v>
+        <v>174513974109.642</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2137,11 +2137,11 @@
         <v>44197</v>
       </c>
       <c r="B99">
-        <v>3781922651</v>
+        <v>28795179085.962</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2155,11 +2155,11 @@
         <v>44197</v>
       </c>
       <c r="B100">
-        <v>10570969868</v>
+        <v>3781922651</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2173,11 +2173,11 @@
         <v>44197</v>
       </c>
       <c r="B101">
-        <v>56260115202.756</v>
+        <v>10570969868</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2191,11 +2191,11 @@
         <v>44197</v>
       </c>
       <c r="B102">
-        <v>74619528755</v>
+        <v>56260115202.756</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2209,11 +2209,11 @@
         <v>44197</v>
       </c>
       <c r="B103">
-        <v>317832124942</v>
+        <v>74619528755</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2227,11 +2227,11 @@
         <v>44197</v>
       </c>
       <c r="B104">
-        <v>87203291188.87</v>
+        <v>317832124942</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Qatar</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2245,11 +2245,11 @@
         <v>44197</v>
       </c>
       <c r="B105">
-        <v>88389728970.91</v>
+        <v>87203291188.87</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Qatar</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2263,11 +2263,11 @@
         <v>44197</v>
       </c>
       <c r="B106">
-        <v>492313790696.653</v>
+        <v>88389728970.91</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Russian Federation</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2281,11 +2281,11 @@
         <v>44197</v>
       </c>
       <c r="B107">
-        <v>1562504482.7</v>
+        <v>492313790696.653</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2299,11 +2299,11 @@
         <v>44197</v>
       </c>
       <c r="B108">
-        <v>34719205.288</v>
+        <v>1562504482.7</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Saint Vincent and the Grenadines</t>
+          <t>Rwanda</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2317,11 +2317,11 @@
         <v>44197</v>
       </c>
       <c r="B109">
-        <v>19174845.703</v>
+        <v>34719205.288</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Sao Tome and Principe</t>
+          <t>Saint Vincent and the Grenadines</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2335,11 +2335,11 @@
         <v>44197</v>
       </c>
       <c r="B110">
-        <v>286467258610.596</v>
+        <v>19174845.703</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Sao Tome and Principe</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2353,11 +2353,11 @@
         <v>44197</v>
       </c>
       <c r="B111">
-        <v>5202221589.634</v>
+        <v>286467258610.596</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Senegal</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2371,11 +2371,11 @@
         <v>44197</v>
       </c>
       <c r="B112">
-        <v>25566160915</v>
+        <v>5202221589.634</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Senegal</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2389,11 +2389,11 @@
         <v>44197</v>
       </c>
       <c r="B113">
-        <v>1951925732.167</v>
+        <v>25566160915</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Seychelles</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2407,11 +2407,11 @@
         <v>44197</v>
       </c>
       <c r="B114">
-        <v>394813673347.297</v>
+        <v>1951925732.167</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Seychelles</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2425,11 +2425,11 @@
         <v>44197</v>
       </c>
       <c r="B115">
-        <v>457081283281.544</v>
+        <v>394813673347.297</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>India</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2443,11 +2443,11 @@
         <v>44197</v>
       </c>
       <c r="B116">
-        <v>104733320881.922</v>
+        <v>457081283281.544</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2461,11 +2461,11 @@
         <v>44197</v>
       </c>
       <c r="B117">
-        <v>335792597810</v>
+        <v>104733320881.922</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Viet Nam</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -2479,11 +2479,11 @@
         <v>44197</v>
       </c>
       <c r="B118">
-        <v>46692128069.11</v>
+        <v>335792597810</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Viet Nam</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -2497,11 +2497,11 @@
         <v>44197</v>
       </c>
       <c r="B119">
-        <v>121321278845.567</v>
+        <v>46692128069.11</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -2515,11 +2515,11 @@
         <v>44197</v>
       </c>
       <c r="B120">
-        <v>6036173160.691</v>
+        <v>121321278845.567</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -2533,11 +2533,11 @@
         <v>44197</v>
       </c>
       <c r="B121">
-        <v>391558519476.67</v>
+        <v>6036173160.691</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -2551,11 +2551,11 @@
         <v>44197</v>
       </c>
       <c r="B122">
-        <v>2291325827.04</v>
+        <v>391558519476.67</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -2569,11 +2569,11 @@
         <v>44197</v>
       </c>
       <c r="B123">
-        <v>2068468810.41</v>
+        <v>2291325827.04</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Suriname</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -2587,11 +2587,11 @@
         <v>44197</v>
       </c>
       <c r="B124">
-        <v>189635063199.877</v>
+        <v>2068468810.41</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Eswatini</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -2605,11 +2605,11 @@
         <v>44197</v>
       </c>
       <c r="B125">
-        <v>379770927042.891</v>
+        <v>189635063199.877</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -2623,11 +2623,11 @@
         <v>44197</v>
       </c>
       <c r="B126">
-        <v>1476799996</v>
+        <v>379770927042.891</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -2641,11 +2641,11 @@
         <v>44197</v>
       </c>
       <c r="B127">
-        <v>266674796256.73</v>
+        <v>1476799996</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Tajikistan</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -2659,11 +2659,11 @@
         <v>44197</v>
       </c>
       <c r="B128">
-        <v>1079792672.912</v>
+        <v>266674796256.73</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -2677,11 +2677,11 @@
         <v>44197</v>
       </c>
       <c r="B129">
-        <v>8620228624.916</v>
+        <v>1079792672.912</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Togo</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -2695,11 +2695,11 @@
         <v>44197</v>
       </c>
       <c r="B130">
-        <v>425159796503.562</v>
+        <v>8620228624.916</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -2713,11 +2713,11 @@
         <v>44197</v>
       </c>
       <c r="B131">
-        <v>16695198641.544</v>
+        <v>425159796503.562</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -2731,11 +2731,11 @@
         <v>44197</v>
       </c>
       <c r="B132">
-        <v>65870275510.39</v>
+        <v>16695198641.544</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -2749,11 +2749,11 @@
         <v>44197</v>
       </c>
       <c r="B133">
-        <v>8186314637.628</v>
+        <v>65870275510.39</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -2767,11 +2767,11 @@
         <v>44197</v>
       </c>
       <c r="B134">
-        <v>40701703944.38</v>
+        <v>8186314637.628</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -2785,11 +2785,11 @@
         <v>44197</v>
       </c>
       <c r="B135">
-        <v>470547786029.463</v>
+        <v>40701703944.38</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -2803,11 +2803,11 @@
         <v>44197</v>
       </c>
       <c r="B136">
-        <v>6390862886.744</v>
+        <v>470547786029.463</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>United Rep. of Tanzania</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -2821,11 +2821,11 @@
         <v>44197</v>
       </c>
       <c r="B137">
-        <v>1753136708106</v>
+        <v>6390862886.744</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United Rep. of Tanzania</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -2839,11 +2839,11 @@
         <v>44197</v>
       </c>
       <c r="B138">
-        <v>5060027958.95</v>
+        <v>1753136708106</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Burkina Faso</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -2857,11 +2857,11 @@
         <v>44197</v>
       </c>
       <c r="B139">
-        <v>9541020289</v>
+        <v>5060027958.95</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Burkina Faso</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -2875,11 +2875,11 @@
         <v>44197</v>
       </c>
       <c r="B140">
-        <v>14092247992.431</v>
+        <v>9541020289</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -2893,11 +2893,11 @@
         <v>44197</v>
       </c>
       <c r="B141">
-        <v>28836585.461</v>
+        <v>14092247992.431</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Samoa</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -2911,14 +2911,32 @@
         <v>44197</v>
       </c>
       <c r="B142">
+        <v>28836585.461</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B143">
         <v>10101351858.32</v>
       </c>
-      <c r="C142" t="inlineStr">
+      <c r="C143" t="inlineStr">
         <is>
           <t>Zambia</t>
         </is>
       </c>
-      <c r="D142" t="inlineStr">
+      <c r="D143" t="inlineStr">
         <is>
           <t>World</t>
         </is>

</xml_diff>